<commit_message>
Demand and Supply of counties
</commit_message>
<xml_diff>
--- a/ClinicCostandCapacity.xlsx
+++ b/ClinicCostandCapacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renzechen/Documents/GitHub/healthcare_calihealth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B45D8A-87FE-1144-8308-38E986749E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B464F2-465E-414B-831A-639701E9E2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="760" windowWidth="30980" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="760" windowWidth="30980" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Square Meteres Available</t>
-  </si>
-  <si>
-    <t>Pop-Up Clinic (Religious Organization, School, Gym, Etc.)</t>
   </si>
   <si>
     <t>outpatient clinic</t>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>Vaccines delivered per square meter, per day</t>
+  </si>
+  <si>
+    <t>Pop-Up Clinic</t>
   </si>
 </sst>
 </file>
@@ -345,7 +345,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -367,7 +367,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -394,7 +394,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>1200</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>1000</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>750</v>
@@ -502,7 +502,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>600</v>
@@ -538,7 +538,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>2000</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>2500</v>
@@ -609,8 +609,8 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="3">
         <v>5000</v>

</xml_diff>